<commit_message>
-m "add p.11 ch8"
</commit_message>
<xml_diff>
--- a/08_portfolio_management/portfolio_example.xlsx
+++ b/08_portfolio_management/portfolio_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ebc00a0f969ad489/Programmazione/github/FromZeroToQuant/FromZeroToQuant-/08_portfolio_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{188DC5AC-8163-4171-86F6-6ECD92B5BED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C0D449-1BA9-4A16-B5F8-DE7647F1E5ED}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{188DC5AC-8163-4171-86F6-6ECD92B5BED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BDE2CE9-D45F-4B74-B5A5-EFEB0E41255E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E60A3A5F-F7BE-4D4D-94AB-E4A3C6B1FB4C}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +778,7 @@
         <v>345.98</v>
       </c>
       <c r="C24">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mod port og ch8, add paper SPY/TLT
</commit_message>
<xml_diff>
--- a/08_portfolio_management/portfolio_example.xlsx
+++ b/08_portfolio_management/portfolio_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ebc00a0f969ad489/Programmazione/github/FromZeroToQuant/FromZeroToQuant-/08_portfolio_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{188DC5AC-8163-4171-86F6-6ECD92B5BED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0EA821CF-5D9A-4F85-A54D-A2B5D6DF7AD8}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{188DC5AC-8163-4171-86F6-6ECD92B5BED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37E99EFB-E854-4BC6-ABBA-CF82B71E2D63}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{E60A3A5F-F7BE-4D4D-94AB-E4A3C6B1FB4C}"/>
   </bookViews>
@@ -169,6 +169,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -503,7 +507,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,7 +778,7 @@
         <v>345.98</v>
       </c>
       <c r="C24">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>